<commit_message>
KPI changes - fix
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2020_06_14/MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/2020_06_14/MARS KPIs.xlsx
@@ -20,22 +20,23 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AE$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AE$69</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$69</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$65</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$65</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$65</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$65</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AE$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$65</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AE$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AE$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AE$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AE$1</definedName>
@@ -51,6 +52,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AE$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AE$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AE$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AE$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5520" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5521" uniqueCount="446">
   <si>
     <t xml:space="preserve">Store type</t>
   </si>
@@ -2044,9 +2046,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="154.935222672065"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.7611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="166.704453441296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.7327935222672"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2269,45 +2270,42 @@
   <dimension ref="A1:AF69"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
-      <selection pane="bottomRight" activeCell="AF69" activeCellId="0" sqref="AF69"/>
+      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="T67" activeCellId="0" sqref="T67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.8825910931174"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9109311740891"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="129.344129554656"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="151.85020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="122.372469635628"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="76.4412955465587"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="49.8178137651822"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="54.1578947368421"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="65.3562753036437"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="64.5587044534413"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="39.6477732793522"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="202.356275303644"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="61.9271255060729"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="56.331983805668"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="33.9352226720648"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="27.3076923076923"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.8542510121458"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="38.5060728744939"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="38.9635627530364"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="28.5668016194332"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="63.6437246963563"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="64.3279352226721"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="41.3603238866397"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="41.8178137651822"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="35.7651821862348"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="57.2429149797571"/>
-    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.3684210526316"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.165991902834"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="139.17004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6234817813765"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="163.506072874494"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="131.627530364372"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="82.2672064777328"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="53.587044534413"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="58.1578947368421"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="70.2712550607288"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="69.4696356275304"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="42.6194331983806"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="217.781376518219"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="66.6153846153846"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="60.5587044534413"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="36.4493927125506"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="29.3643724696356"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.995951417004"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="41.4777327935223"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="41.9352226720648"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="30.7368421052632"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="68.4412955465587"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="69.2429149797571"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="44.4453441295547"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="44.9028340080972"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="38.5060728744939"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="61.587044534413"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3032,10 +3030,10 @@
         <v>4607065372217</v>
       </c>
       <c r="R10" s="13"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11" t="s">
+      <c r="S10" s="11" t="s">
         <v>68</v>
       </c>
+      <c r="T10" s="11"/>
       <c r="U10" s="13"/>
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
@@ -6964,7 +6962,9 @@
         <v>6048</v>
       </c>
       <c r="R66" s="11"/>
-      <c r="S66" s="11"/>
+      <c r="S66" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="T66" s="11"/>
       <c r="U66" s="11"/>
       <c r="V66" s="11"/>
@@ -7030,10 +7030,10 @@
         <v>248</v>
       </c>
       <c r="R67" s="11"/>
-      <c r="S67" s="11"/>
-      <c r="T67" s="11" t="s">
+      <c r="S67" s="11" t="s">
         <v>68</v>
       </c>
+      <c r="T67" s="11"/>
       <c r="U67" s="11"/>
       <c r="V67" s="11"/>
       <c r="W67" s="11"/>
@@ -7104,10 +7104,10 @@
         <v>4607065739164</v>
       </c>
       <c r="R68" s="11"/>
-      <c r="S68" s="11"/>
-      <c r="T68" s="11" t="s">
+      <c r="S68" s="14" t="s">
         <v>68</v>
       </c>
+      <c r="T68" s="11"/>
       <c r="U68" s="11"/>
       <c r="V68" s="11"/>
       <c r="W68" s="11"/>
@@ -7175,10 +7175,10 @@
         <v>254</v>
       </c>
       <c r="R69" s="14"/>
-      <c r="S69" s="14"/>
-      <c r="T69" s="14" t="s">
+      <c r="S69" s="14" t="s">
         <v>68</v>
       </c>
+      <c r="T69" s="14"/>
       <c r="U69" s="14"/>
       <c r="V69" s="14"/>
       <c r="W69" s="14"/>
@@ -7196,7 +7196,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE69"/>
+  <autoFilter ref="A1:AE1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -7217,41 +7217,38 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AF2" activeCellId="0" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3238866396761"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.8825910931174"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9109311740891"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="85.2388663967611"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.6518218623482"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="151.85020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="172.761133603239"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="50.7327935222672"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="49.8178137651822"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="54.1578947368421"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="65.3562753036437"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="64.5587044534413"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="39.6477732793522"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="54.1578947368421"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="61.9271255060729"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="56.331983805668"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.165991902834"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="27.3076923076923"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.8542510121458"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="38.5060728744939"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="38.9635627530364"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="34.2793522267206"/>
-    <col collapsed="false" hidden="false" max="31" min="26" style="0" width="52.4453441295547"/>
-    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6234817813765"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.3684210526316"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.165991902834"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="91.748987854251"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.4817813765182"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="163.506072874494"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="186.016194331984"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="54.6153846153846"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="53.587044534413"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="58.1578947368421"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="70.2712550607288"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="69.4696356275304"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="42.6194331983806"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="58.1578947368421"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="66.6153846153846"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="60.5587044534413"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="32.336032388664"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="29.3643724696356"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.995951417004"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="41.4777327935223"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="41.9352226720648"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="36.9068825910931"/>
+    <col collapsed="false" hidden="false" max="31" min="26" style="0" width="56.4453441295547"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8561,15 +8558,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="119.744939271255"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="34.0485829959514"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.3076923076923"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="119.744939271255"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="32.336032388664"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="69.3562753036437"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="128.886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="36.5627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6518218623482"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.3643724696356"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="128.886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="34.7368421052632"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="74.6113360323887"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27604,10 +27601,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.0202429149798"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="76.0971659919028"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7611336032389"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="81.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29420,9 +29418,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.8987854251012"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8137651821862"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29490,9 +29487,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4736842105263"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9028340080972"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29551,10 +29546,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.7611336032389"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="165.562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.2186234817814"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.7327935222672"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="178.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.2145748987854"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29745,11 +29739,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.5587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.4736842105263"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.5587044534413"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.7854251012146"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.4696356275304"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="80.8947368421053"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>